<commit_message>
Notebook clean up, wet lab work
</commit_message>
<xml_diff>
--- a/notebooks/t7/rounds/T7_Round1.xlsx
+++ b/notebooks/t7/rounds/T7_Round1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaiyi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteodibernardo/Documents/GitHub/directed_evolution/notebooks/t7/rounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B63B29FA-C1B6-A74F-B013-822ADECF0D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15D8DDE-A24F-5A49-B5B3-B3AD65CD6364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{B4658473-2CB0-7743-9E6A-3AC6FA0C41B3}"/>
+    <workbookView xWindow="1420" yWindow="760" windowWidth="28040" windowHeight="16280" xr2:uid="{B4658473-2CB0-7743-9E6A-3AC6FA0C41B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateCount="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,37 +37,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>T7pol_12N</t>
-  </si>
-  <si>
-    <t>T7pol_25N</t>
-  </si>
-  <si>
-    <t>T7pol_WT</t>
-  </si>
-  <si>
-    <t>T7pol_89R</t>
-  </si>
-  <si>
-    <t>T7pol_134T</t>
-  </si>
-  <si>
-    <t>T7pol_177L</t>
-  </si>
-  <si>
-    <t>T7pol_225E</t>
-  </si>
-  <si>
-    <t>T7pol_241W</t>
-  </si>
-  <si>
-    <t>T7pol_273H</t>
-  </si>
-  <si>
     <t>Variant</t>
   </si>
   <si>
-    <t>Effect vector</t>
+    <t>12N</t>
+  </si>
+  <si>
+    <t>25N</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>89R</t>
+  </si>
+  <si>
+    <t>134T</t>
+  </si>
+  <si>
+    <t>177L</t>
+  </si>
+  <si>
+    <t>225E</t>
+  </si>
+  <si>
+    <t>241W</t>
+  </si>
+  <si>
+    <t>273H</t>
+  </si>
+  <si>
+    <t>fitness</t>
   </si>
 </sst>
 </file>
@@ -431,7 +430,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +440,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -449,7 +448,7 @@
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1.0738461252709337</v>
@@ -457,7 +456,7 @@
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0.67722656175809492</v>
@@ -465,7 +464,7 @@
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0.999999999999999</v>
@@ -473,7 +472,7 @@
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0.7404994870212519</v>
@@ -481,7 +480,7 @@
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1.0748909968196614</v>
@@ -489,7 +488,7 @@
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1.042705614158187</v>
@@ -497,7 +496,7 @@
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1.0758613629099871</v>
@@ -505,7 +504,7 @@
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.93835109865527855</v>
@@ -513,7 +512,7 @@
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.78514726854608041</v>

</xml_diff>